<commit_message>
Add steps and tests
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -13,11 +13,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Набор тест-кейсов'!$A$1:$H$68</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="219">
   <si>
     <t>Описание( Summary):</t>
   </si>
@@ -1076,9 +1077,6 @@
     <t>1. Заполнить поле "Логин" - LOGIN1
 2. Заполнить поле "Пароль" - password2
 3. Нажать на кнопку "ВОЙТИ"</t>
-  </si>
-  <si>
-    <t>Уведомления нет</t>
   </si>
   <si>
     <t>Не пройден                                    Причина: элемент не кликабелен.</t>
@@ -2544,7 +2542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2558,8 +2556,8 @@
   <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3111,11 +3109,9 @@
         <v>166</v>
       </c>
       <c r="G24" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="H24" s="105" t="s">
-        <v>217</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="H24" s="105"/>
     </row>
     <row r="25" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A25" s="47">
@@ -3137,9 +3133,7 @@
       <c r="G25" s="62" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="105" t="s">
-        <v>217</v>
-      </c>
+      <c r="H25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A26" s="46">
@@ -3161,9 +3155,7 @@
       <c r="G26" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="H26" s="105" t="s">
-        <v>217</v>
-      </c>
+      <c r="H26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="84" x14ac:dyDescent="0.2">
       <c r="A27" s="47">
@@ -3230,7 +3222,7 @@
         <v>159</v>
       </c>
       <c r="H29" s="107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="84" x14ac:dyDescent="0.2">
@@ -3385,7 +3377,9 @@
       <c r="G36" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="H36" s="104"/>
+      <c r="H36" s="104" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="131.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48">
@@ -3408,7 +3402,7 @@
         <v>192</v>
       </c>
       <c r="H37" s="107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="24" x14ac:dyDescent="0.2">
@@ -3964,7 +3958,7 @@
         <v>119</v>
       </c>
       <c r="H62" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="96" x14ac:dyDescent="0.2">

</xml_diff>